<commit_message>
Added and updated test data
</commit_message>
<xml_diff>
--- a/testdata/excel/testdata.xlsx
+++ b/testdata/excel/testdata.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7635"/>
   </bookViews>
   <sheets>
-    <sheet name="STAG_ExcelDataTest" sheetId="1" r:id="rId1"/>
+    <sheet name="QA_ExcelDataTest" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -398,7 +398,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>